<commit_message>
small addition to raw files
</commit_message>
<xml_diff>
--- a/tests/data/mbe/2023_06_12/MBE8_config.xlsx
+++ b/tests/data/mbe/2023_06_12/MBE8_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MBE sources" sheetId="1" state="visible" r:id="rId3"/>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="177">
   <si>
     <t xml:space="preserve"># meaning</t>
   </si>
@@ -505,13 +505,35 @@
     <t xml:space="preserve">SUB</t>
   </si>
   <si>
+    <t xml:space="preserve">Sub</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sub.PID.MV</t>
   </si>
   <si>
     <t xml:space="preserve">Sub.PID.wOP</t>
   </si>
   <si>
-    <t xml:space="preserve">date  of gas mixing config. Note: this date must be preceding the growth experiment start!</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date  of gas mixing config. Note: this date must be preceding the growth start time! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The start time is calculated checking when the MFC of the gases exceed the threshold number included in “MBE config files” sheet</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">date  of gas mixing config. Note: this date must be preceding the growth start time! The start time is calculated checking when the MFC of the gases exceed the threshold number included in “MBE config files” sheet</t>
   </si>
   <si>
     <t xml:space="preserve">initials of grower(s)</t>
@@ -520,6 +542,9 @@
     <t xml:space="preserve">serial number of port of affected plasma source</t>
   </si>
   <si>
+    <t xml:space="preserve">threshold to establish that a MFC is open </t>
+  </si>
+  <si>
     <t xml:space="preserve">Mass flow measurement</t>
   </si>
   <si>
@@ -545,6 +570,9 @@
   </si>
   <si>
     <t xml:space="preserve">mfc_range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfc_threshold</t>
   </si>
   <si>
     <t xml:space="preserve">mfc_gas</t>
@@ -721,7 +749,7 @@
     <numFmt numFmtId="171" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="172" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -771,6 +799,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -832,6 +865,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
@@ -840,12 +879,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF77BC65"/>
         <bgColor rgb="FF92D050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
     <fill>
@@ -932,7 +965,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="104">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1129,6 +1162,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1145,6 +1182,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1165,6 +1206,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1193,11 +1238,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1205,7 +1254,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1234,26 +1283,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1261,11 +1290,31 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1273,15 +1322,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1289,16 +1334,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1313,18 +1350,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1337,23 +1366,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1362,18 +1379,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1628,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:AW49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2216,7 +2221,9 @@
       <c r="P8" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="Q8" s="42"/>
+      <c r="Q8" s="42" t="s">
+        <v>73</v>
+      </c>
       <c r="R8" s="41" t="s">
         <v>85</v>
       </c>
@@ -2305,7 +2312,9 @@
       <c r="P9" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="Q9" s="42"/>
+      <c r="Q9" s="42" t="s">
+        <v>73</v>
+      </c>
       <c r="R9" s="41" t="s">
         <v>94</v>
       </c>
@@ -2389,7 +2398,9 @@
       <c r="P10" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="Q10" s="42"/>
+      <c r="Q10" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="R10" s="42" t="s">
         <v>99</v>
       </c>
@@ -2464,15 +2475,20 @@
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
       <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
+      <c r="Q11" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="R11" s="41" t="s">
+        <v>106</v>
+      </c>
       <c r="T11" s="41" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U11" s="41" t="s">
         <v>76</v>
       </c>
       <c r="V11" s="41" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W11" s="41" t="s">
         <v>78</v>
@@ -2939,91 +2955,95 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ35"/>
+  <dimension ref="A1:AR35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="47" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="17.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="47" width="19.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="48" width="13.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="48" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="48" width="13.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="48" width="11.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="48" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="48" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="48" width="15.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="48" width="5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="39" min="13" style="48" width="10.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="44" style="48" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="48" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="49" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="48" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="48" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="48" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="48" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="48" width="5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="14" style="48" width="10.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="45" style="48" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="48" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="52" customFormat="true" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="53" customFormat="true" ht="175.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="H1" s="50" t="s">
+        <v>113</v>
+      </c>
       <c r="I1" s="6"/>
-      <c r="J1" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="50" t="s">
+        <v>115</v>
+      </c>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="51"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="8"/>
       <c r="AC1" s="6"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="9"/>
       <c r="AF1" s="6"/>
       <c r="AG1" s="6"/>
       <c r="AH1" s="6"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="10"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="7"/>
       <c r="AK1" s="10"/>
-      <c r="AL1" s="6"/>
+      <c r="AL1" s="10"/>
       <c r="AM1" s="6"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-    </row>
-    <row r="2" s="53" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
+    </row>
+    <row r="2" s="55" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
@@ -3033,12 +3053,14 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -3055,79 +3077,81 @@
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="15"/>
       <c r="AC2" s="13"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="16"/>
       <c r="AF2" s="13"/>
       <c r="AG2" s="13"/>
       <c r="AH2" s="13"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="17"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="14"/>
       <c r="AK2" s="17"/>
-      <c r="AL2" s="13"/>
+      <c r="AL2" s="17"/>
       <c r="AM2" s="13"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-    </row>
-    <row r="3" s="56" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="52"/>
+      <c r="AQ2" s="52"/>
+      <c r="AR2" s="52"/>
+    </row>
+    <row r="3" s="58" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="55" t="s">
-        <v>115</v>
+      <c r="D3" s="57" t="s">
+        <v>118</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55"/>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="55"/>
-      <c r="AI3" s="55"/>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="55"/>
-      <c r="AM3" s="55"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AP3" s="51"/>
-      <c r="AQ3" s="51"/>
-    </row>
-    <row r="4" s="62" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L3" s="20"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57"/>
+      <c r="AD3" s="57"/>
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="57"/>
+      <c r="AJ3" s="57"/>
+      <c r="AK3" s="57"/>
+      <c r="AL3" s="57"/>
+      <c r="AM3" s="57"/>
+      <c r="AN3" s="57"/>
+      <c r="AO3" s="52"/>
+      <c r="AP3" s="52"/>
+      <c r="AQ3" s="52"/>
+      <c r="AR3" s="52"/>
+    </row>
+    <row r="4" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>35</v>
       </c>
@@ -3137,13 +3161,13 @@
       <c r="C4" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>116</v>
+      <c r="D4" s="59" t="s">
+        <v>119</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
@@ -3161,87 +3185,89 @@
       <c r="W4" s="28"/>
       <c r="X4" s="28"/>
       <c r="Y4" s="28"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="62"/>
       <c r="AC4" s="28"/>
-      <c r="AD4" s="60"/>
-      <c r="AE4" s="28"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="63"/>
       <c r="AF4" s="28"/>
       <c r="AG4" s="28"/>
       <c r="AH4" s="28"/>
-      <c r="AI4" s="58"/>
+      <c r="AI4" s="28"/>
       <c r="AJ4" s="61"/>
-      <c r="AK4" s="61"/>
-      <c r="AL4" s="28"/>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
       <c r="AM4" s="28"/>
-      <c r="AN4" s="51"/>
-      <c r="AO4" s="51"/>
-      <c r="AP4" s="51"/>
-      <c r="AQ4" s="51"/>
-    </row>
-    <row r="5" s="52" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AN4" s="28"/>
+      <c r="AO4" s="52"/>
+      <c r="AP4" s="52"/>
+      <c r="AQ4" s="52"/>
+      <c r="AR4" s="52"/>
+    </row>
+    <row r="5" s="53" customFormat="true" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64" t="s">
+      <c r="F5" s="67"/>
+      <c r="G5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="68"/>
+      <c r="I5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="J5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="64"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="65"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="65"/>
-      <c r="AH5" s="65"/>
-      <c r="AI5" s="65"/>
-      <c r="AJ5" s="65"/>
-      <c r="AK5" s="65"/>
-      <c r="AL5" s="65"/>
-      <c r="AM5" s="65"/>
-      <c r="AN5" s="51"/>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-    </row>
-    <row r="6" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
+      <c r="Y5" s="67"/>
+      <c r="Z5" s="67"/>
+      <c r="AA5" s="67"/>
+      <c r="AB5" s="69"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="69"/>
+      <c r="AI5" s="69"/>
+      <c r="AJ5" s="69"/>
+      <c r="AK5" s="69"/>
+      <c r="AL5" s="69"/>
+      <c r="AM5" s="69"/>
+      <c r="AN5" s="69"/>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+    </row>
+    <row r="6" s="70" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
         <v>40</v>
       </c>
@@ -3252,33 +3278,35 @@
         <v>26</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>123</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L6" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="34"/>
       <c r="N6" s="34"/>
       <c r="O6" s="34"/>
       <c r="P6" s="34"/>
@@ -3291,350 +3319,371 @@
       <c r="W6" s="34"/>
       <c r="X6" s="34"/>
       <c r="Y6" s="34"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="36"/>
-      <c r="AB6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="35"/>
+      <c r="AB6" s="36"/>
       <c r="AC6" s="34"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="34"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="37"/>
       <c r="AF6" s="34"/>
       <c r="AG6" s="34"/>
       <c r="AH6" s="34"/>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="38"/>
+      <c r="AI6" s="34"/>
+      <c r="AJ6" s="35"/>
       <c r="AK6" s="38"/>
-      <c r="AL6" s="34"/>
+      <c r="AL6" s="38"/>
       <c r="AM6" s="34"/>
-      <c r="AN6" s="51"/>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
+      <c r="AN6" s="34"/>
+      <c r="AO6" s="52"/>
+      <c r="AP6" s="52"/>
+      <c r="AQ6" s="52"/>
+      <c r="AR6" s="52"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="68" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="48" t="n">
+        <v>4</v>
       </c>
       <c r="F7" s="48" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="K7" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="L7" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="W7" s="69"/>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
+        <v>131</v>
+      </c>
+      <c r="H7" s="49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="L7" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="73"/>
+      <c r="V7" s="73"/>
+      <c r="W7" s="73"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="73"/>
+      <c r="Z7" s="73"/>
+      <c r="AA7" s="73"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="48" t="n">
+        <v>4</v>
       </c>
       <c r="F8" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="69" t="s">
+      <c r="G8" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="49" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I8" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="J8" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="K8" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="69"/>
+      <c r="K8" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="L8" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="73"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="68" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="48" t="n">
+        <v>4</v>
       </c>
       <c r="F9" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="69" t="s">
+      <c r="I9" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="70"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="68" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="48" t="n">
+        <v>4</v>
       </c>
       <c r="F10" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="J10" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="K10" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="I10" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="L10" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="74"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="69"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="70"/>
+      <c r="C11" s="71"/>
+      <c r="G11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="69"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="G12" s="73"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="74"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="69"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="70"/>
+      <c r="G13" s="73"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="N13" s="76"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="76"/>
+      <c r="Q13" s="74"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="69"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="70"/>
+      <c r="G14" s="73"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+      <c r="N14" s="76"/>
+      <c r="O14" s="76"/>
+      <c r="P14" s="76"/>
+      <c r="Q14" s="74"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="69"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
+      <c r="G15" s="73"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="69"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="P16" s="70"/>
+      <c r="G16" s="73"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="Q16" s="74"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="69"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="P17" s="70"/>
+      <c r="G17" s="73"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="Q17" s="74"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="69"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="70"/>
+      <c r="G18" s="73"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+      <c r="P18" s="76"/>
+      <c r="Q18" s="74"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="69"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="P19" s="70"/>
-      <c r="X19" s="74"/>
+      <c r="G19" s="73"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="Q19" s="74"/>
+      <c r="Y19" s="78"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
-      <c r="P20" s="70"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="Q20" s="74"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="P21" s="70"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="Q21" s="74"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="P22" s="70"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="Q22" s="74"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="70"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="P23" s="76"/>
+      <c r="Q23" s="74"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="P24" s="70"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="Q24" s="74"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="P25" s="70"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="Q25" s="74"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="P26" s="70"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="Q26" s="74"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="P27" s="70"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
+      <c r="Q27" s="74"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="P28" s="70"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="Q28" s="74"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="P29" s="70"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="Q29" s="74"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="P30" s="70"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="Q30" s="74"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="P31" s="70"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="Q31" s="74"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="P32" s="70"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="Q32" s="74"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D10" type="list">
+      <formula1>#ref!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G13:G19" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q7:Q10 P11:P14 P16:P32" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:R10 Q11:Q14 Q16:Q32" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D10" type="list">
-      <formula1>#ref!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H7:H10 G11:G12" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I7:I10 G11:G12" type="list">
       <formula1>'MBE chamber env'!$C$7:$C$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3657,148 +3706,148 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="3" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="3" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="49" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="50" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="75"/>
-    </row>
-    <row r="2" s="77" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="76" t="s">
+      <c r="D1" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="79"/>
+    </row>
+    <row r="2" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="78"/>
-    </row>
-    <row r="3" s="56" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="82"/>
+    </row>
+    <row r="3" s="58" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="79"/>
-    </row>
-    <row r="4" s="62" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="83"/>
+    </row>
+    <row r="4" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="80"/>
-    </row>
-    <row r="5" s="82" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="81" t="s">
+      <c r="J4" s="84"/>
+    </row>
+    <row r="5" s="86" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="83"/>
+      <c r="J5" s="87"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="85" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="85" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="85" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="85" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="85" t="s">
+      <c r="B6" s="89" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="85" t="s">
+      <c r="C6" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="85"/>
+      <c r="D6" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="89" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="89" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="87" t="s">
-        <v>150</v>
-      </c>
-      <c r="C7" s="88" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="87" t="s">
-        <v>152</v>
-      </c>
-      <c r="E7" s="88" t="s">
-        <v>151</v>
+      <c r="B7" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="91" t="s">
+        <v>155</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
+        <v>155</v>
+      </c>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
+      <c r="C8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
+      <c r="C9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
+      <c r="C10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3816,109 +3865,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="89" width="15.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="15.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="1" s="92" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="93" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
     </row>
     <row r="2" s="96" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-    </row>
-    <row r="3" s="98" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" s="97" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-    </row>
-    <row r="4" s="102" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="99" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+    </row>
+    <row r="4" s="100" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-    </row>
-    <row r="5" s="104" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="81" t="s">
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+    </row>
+    <row r="5" s="101" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-    </row>
-    <row r="6" s="106" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="66" t="s">
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+    </row>
+    <row r="6" s="102" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="89" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="89" t="s">
+      <c r="C7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E7" s="3" t="n">
@@ -3946,8 +3982,8 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3960,71 +3996,71 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="3" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="49" customFormat="true" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="50" customFormat="true" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" s="53" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="55" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="13" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" s="56" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="58" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="G3" s="56" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" s="62" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" s="65" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>35</v>
       </c>
@@ -4034,27 +4070,27 @@
       <c r="C4" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="57"/>
-    </row>
-    <row r="5" s="82" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="59"/>
+    </row>
+    <row r="5" s="86" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="64"/>
-    </row>
-    <row r="6" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="67"/>
+    </row>
+    <row r="6" s="70" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
         <v>40</v>
       </c>
@@ -4065,87 +4101,87 @@
         <v>26</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>163</v>
-      </c>
-      <c r="G6" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" s="66" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="J6" s="66" t="s">
+      <c r="F6" s="70" t="s">
         <v>167</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="J6" s="70" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="46"/>
       <c r="B7" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="68"/>
+        <v>128</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="72"/>
       <c r="F7" s="3" t="n">
         <v>456</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="46"/>
       <c r="B8" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="68"/>
+        <v>128</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="72"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="46"/>
       <c r="B9" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="68"/>
+        <v>137</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="72"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="46"/>
       <c r="B10" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="68"/>
+        <v>137</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="72"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4172,63 +4208,63 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="107" width="14.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="87" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="103" width="14.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="49" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="50" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="108" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="54" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" s="55" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="57" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" s="109" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="60" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" s="110" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="81" t="s">
+    <row r="5" s="68" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="85" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="66" t="s">
+    <row r="6" s="70" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="66" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="66" t="s">
+      <c r="B6" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="87" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" s="87" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" s="87" t="s">
+      <c r="B7" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="49" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sample status and source length
</commit_message>
<xml_diff>
--- a/tests/data/mbe/2023_06_12/MBE8_config.xlsx
+++ b/tests/data/mbe/2023_06_12/MBE8_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="MBE sources" sheetId="1" state="visible" r:id="rId3"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="179">
   <si>
     <t xml:space="preserve"># meaning</t>
   </si>
@@ -208,6 +208,9 @@
     <t xml:space="preserve">diameter of source orifice</t>
   </si>
   <si>
+    <t xml:space="preserve">the length of the source</t>
+  </si>
+  <si>
     <t xml:space="preserve">polar angle of flux vector out of source</t>
   </si>
   <si>
@@ -316,7 +319,13 @@
     <t xml:space="preserve">port_diameter</t>
   </si>
   <si>
-    <t xml:space="preserve">distance</t>
+    <t xml:space="preserve">port to sub distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source length</t>
   </si>
   <si>
     <t xml:space="preserve">theta</t>
@@ -512,25 +521,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sub.PID.wOP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">date  of gas mixing config. Note: this date must be preceding the growth start time! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The start time is calculated checking when the MFC of the gases exceed the threshold number included in “MBE config files” sheet</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">date  of gas mixing config. Note: this date must be preceding the growth start time! The start time is calculated checking when the MFC of the gases exceed the threshold number included in “MBE config files” sheet</t>
@@ -749,7 +739,7 @@
     <numFmt numFmtId="171" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="172" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -799,11 +789,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1246,7 +1231,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1322,7 +1307,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1631,10 +1616,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AW49"/>
+  <dimension ref="A1:AX49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1644,29 +1629,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="13.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="3" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="29.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="18.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="3" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="3" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="15.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="3" width="17.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="3" width="13.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="3" width="11.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="33" style="3" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="21.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="18.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="3" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="24.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="3" width="14.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="3" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="3" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="3" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="3" width="13.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="32" style="3" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="3" width="11.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="34" style="3" width="10.54"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="102.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,17 +1684,17 @@
       <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>10</v>
@@ -1716,12 +1703,12 @@
         <v>11</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="W1" s="6" t="s">
@@ -1754,116 +1741,124 @@
       <c r="AF1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="8"/>
-      <c r="AN1" s="9"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="10"/>
+      <c r="AG1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="8"/>
+      <c r="AO1" s="9"/>
+      <c r="AT1" s="7"/>
       <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
     </row>
     <row r="2" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" s="13" t="s">
         <v>29</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="15"/>
-      <c r="AN2" s="16"/>
-      <c r="AS2" s="14"/>
-      <c r="AT2" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="15"/>
+      <c r="AO2" s="16"/>
+      <c r="AT2" s="14"/>
       <c r="AU2" s="17"/>
+      <c r="AV2" s="17"/>
     </row>
     <row r="3" s="20" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="E3" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="J3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="23"/>
-      <c r="AN3" s="24"/>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="25"/>
+      <c r="O3" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="23"/>
+      <c r="AO3" s="24"/>
+      <c r="AT3" s="22"/>
       <c r="AU3" s="25"/>
+      <c r="AV3" s="25"/>
     </row>
     <row r="4" s="28" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="26"/>
+        <v>38</v>
+      </c>
       <c r="J4" s="26"/>
       <c r="K4" s="26"/>
-      <c r="M4" s="26"/>
+      <c r="L4" s="26"/>
       <c r="N4" s="26"/>
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
@@ -1900,50 +1895,51 @@
       <c r="AU4" s="26"/>
       <c r="AV4" s="26"/>
       <c r="AW4" s="26"/>
+      <c r="AX4" s="26"/>
     </row>
     <row r="5" s="29" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H5" s="31"/>
       <c r="I5" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="31"/>
       <c r="L5" s="31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="Q5" s="31"/>
       <c r="R5" s="31"/>
       <c r="S5" s="31"/>
@@ -1964,129 +1960,133 @@
       <c r="AH5" s="31"/>
       <c r="AI5" s="31"/>
       <c r="AJ5" s="31"/>
+      <c r="AK5" s="31"/>
     </row>
     <row r="6" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N6" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O6" s="34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R6" s="34" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="S6" s="34" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="T6" s="34" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="V6" s="34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W6" s="34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="X6" s="34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Y6" s="34" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Z6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA6" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB6" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="AA6" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB6" s="34" t="s">
-        <v>63</v>
-      </c>
       <c r="AC6" s="34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AD6" s="34" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AE6" s="34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AF6" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG6" s="34"/>
+        <v>69</v>
+      </c>
+      <c r="AG6" s="34" t="s">
+        <v>24</v>
+      </c>
       <c r="AH6" s="34"/>
       <c r="AI6" s="34"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="36"/>
-      <c r="AL6" s="34"/>
+      <c r="AJ6" s="34"/>
+      <c r="AK6" s="35"/>
+      <c r="AL6" s="36"/>
       <c r="AM6" s="34"/>
-      <c r="AN6" s="37"/>
-      <c r="AO6" s="34"/>
+      <c r="AN6" s="34"/>
+      <c r="AO6" s="37"/>
       <c r="AP6" s="34"/>
       <c r="AQ6" s="34"/>
       <c r="AR6" s="34"/>
-      <c r="AS6" s="35"/>
-      <c r="AT6" s="38"/>
+      <c r="AS6" s="34"/>
+      <c r="AT6" s="35"/>
       <c r="AU6" s="38"/>
-      <c r="AV6" s="34"/>
+      <c r="AV6" s="38"/>
       <c r="AW6" s="34"/>
+      <c r="AX6" s="34"/>
     </row>
     <row r="7" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39"/>
       <c r="B7" s="40" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D7" s="41" t="n">
         <v>1</v>
@@ -2095,94 +2095,97 @@
         <v>34</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>4</v>
+        <v>245</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="H7" s="42" t="n">
+      <c r="H7" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="I7" s="42" t="n">
         <v>40</v>
       </c>
-      <c r="I7" s="42" t="n">
+      <c r="J7" s="42" t="n">
         <v>132</v>
       </c>
-      <c r="J7" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="M7" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="N7" s="42" t="n">
+      <c r="K7" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="43"/>
+      <c r="M7" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="42" t="n">
         <v>45</v>
       </c>
-      <c r="O7" s="42" t="s">
-        <v>71</v>
-      </c>
       <c r="P7" s="42" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q7" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="R7" s="43" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="R7" s="42" t="s">
+        <v>76</v>
       </c>
       <c r="S7" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="T7" s="41" t="s">
-        <v>75</v>
+      <c r="T7" s="43" t="s">
+        <v>77</v>
       </c>
       <c r="U7" s="41" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="V7" s="41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="W7" s="41" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="X7" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y7" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z7" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="Y7" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z7" s="41" t="s">
-        <v>80</v>
-      </c>
       <c r="AA7" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB7" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC7" s="43" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AD7" s="43" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AE7" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF7" s="43"/>
+        <v>84</v>
+      </c>
+      <c r="AF7" s="43" t="s">
+        <v>84</v>
+      </c>
       <c r="AG7" s="43"/>
       <c r="AH7" s="43"/>
       <c r="AI7" s="43"/>
       <c r="AJ7" s="43"/>
+      <c r="AK7" s="43"/>
     </row>
     <row r="8" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="B8" s="40" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D8" s="41" t="n">
         <v>2</v>
@@ -2191,89 +2194,92 @@
         <v>45</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>4</v>
+        <v>246</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="H8" s="42" t="n">
+      <c r="H8" s="3" t="n">
+        <v>124</v>
+      </c>
+      <c r="I8" s="42" t="n">
         <v>21</v>
       </c>
-      <c r="I8" s="42" t="n">
+      <c r="J8" s="42" t="n">
         <v>64</v>
       </c>
-      <c r="J8" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>83</v>
+      <c r="K8" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="40"/>
+      <c r="M8" s="41" t="s">
+        <v>85</v>
       </c>
       <c r="N8" s="42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O8" s="42" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="R8" s="41" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="R8" s="42" t="s">
+        <v>76</v>
       </c>
       <c r="S8" s="41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="T8" s="41" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="U8" s="41" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="V8" s="41" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="W8" s="41" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="X8" s="41" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y8" s="41" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="Z8" s="41" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AA8" s="41" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="AB8" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC8" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AD8" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AE8" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="AF8" s="41" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
       <c r="B9" s="40" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D9" s="41" t="n">
         <v>3</v>
@@ -2282,86 +2288,89 @@
         <v>56</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>4</v>
+        <v>247</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="H9" s="42" t="n">
+      <c r="H9" s="3" t="n">
+        <v>125</v>
+      </c>
+      <c r="I9" s="42" t="n">
         <v>21</v>
       </c>
-      <c r="I9" s="42" t="n">
+      <c r="J9" s="42" t="n">
         <v>116</v>
       </c>
-      <c r="J9" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="M9" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="N9" s="42" t="n">
+      <c r="K9" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="O9" s="42" t="n">
         <v>56</v>
       </c>
-      <c r="O9" s="42" t="s">
-        <v>94</v>
-      </c>
       <c r="P9" s="42" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="Q9" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="R9" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="T9" s="41" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="R9" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="41" t="s">
+        <v>97</v>
       </c>
       <c r="U9" s="41" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="V9" s="41" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="W9" s="41" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="X9" s="41" t="s">
         <v>81</v>
       </c>
       <c r="Y9" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA9" s="41" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="Z9" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="AB9" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC9" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AD9" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AE9" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="AF9" s="41" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="B10" s="40" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D10" s="41" t="n">
         <v>4</v>
@@ -2370,84 +2379,87 @@
         <v>67</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>4</v>
+        <v>248</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="H10" s="42" t="n">
+      <c r="H10" s="3" t="n">
+        <v>126</v>
+      </c>
+      <c r="I10" s="42" t="n">
         <v>330</v>
       </c>
-      <c r="I10" s="42" t="n">
+      <c r="J10" s="42" t="n">
         <v>180</v>
       </c>
-      <c r="J10" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42" t="s">
-        <v>99</v>
-      </c>
+      <c r="K10" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="42"/>
       <c r="P10" s="42" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="Q10" s="42" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="R10" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="T10" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="S10" s="42" t="s">
+        <v>102</v>
       </c>
       <c r="U10" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="V10" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="W10" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="X10" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Y10" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA10" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="Z10" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="AB10" s="41" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="AC10" s="41" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD10" s="41" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE10" s="41" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="AF10" s="41" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="39"/>
       <c r="B11" s="40" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D11" s="41" t="n">
         <v>5</v>
@@ -2456,66 +2468,69 @@
         <v>78</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>4</v>
+        <v>249</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="H11" s="42" t="n">
+      <c r="H11" s="3" t="n">
+        <v>127</v>
+      </c>
+      <c r="I11" s="42" t="n">
         <v>180</v>
       </c>
-      <c r="I11" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="K11" s="40"/>
-      <c r="M11" s="42"/>
+      <c r="J11" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="40"/>
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
       <c r="P11" s="42"/>
-      <c r="Q11" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="R11" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="T11" s="41" t="s">
-        <v>107</v>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" s="41" t="s">
+        <v>109</v>
       </c>
       <c r="U11" s="41" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="V11" s="41" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="W11" s="41" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="X11" s="41" t="s">
         <v>81</v>
       </c>
       <c r="Y11" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA11" s="41" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="Z11" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="AB11" s="41" t="s">
         <v>81</v>
       </c>
       <c r="AC11" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AD11" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AE11" s="41" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="AF11" s="41" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,16 +2539,17 @@
       <c r="C12" s="40"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="40"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
-      <c r="M12" s="42"/>
+      <c r="L12" s="40"/>
       <c r="N12" s="42"/>
       <c r="O12" s="42"/>
       <c r="P12" s="42"/>
       <c r="Q12" s="42"/>
-      <c r="Z12" s="3"/>
+      <c r="R12" s="42"/>
+      <c r="AA12" s="3"/>
     </row>
     <row r="13" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
@@ -2541,16 +2557,17 @@
       <c r="C13" s="40"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="40"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
-      <c r="M13" s="42"/>
+      <c r="L13" s="40"/>
       <c r="N13" s="42"/>
       <c r="O13" s="42"/>
       <c r="P13" s="42"/>
       <c r="Q13" s="42"/>
-      <c r="Z13" s="3"/>
+      <c r="R13" s="42"/>
+      <c r="AA13" s="3"/>
     </row>
     <row r="14" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
@@ -2558,15 +2575,16 @@
       <c r="C14" s="40"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="I14" s="40"/>
+      <c r="H14" s="3"/>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
-      <c r="M14" s="42"/>
+      <c r="L14" s="40"/>
       <c r="N14" s="42"/>
       <c r="O14" s="42"/>
       <c r="P14" s="42"/>
       <c r="Q14" s="42"/>
-      <c r="Z14" s="3"/>
+      <c r="R14" s="42"/>
+      <c r="AA14" s="3"/>
     </row>
     <row r="15" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39"/>
@@ -2574,15 +2592,16 @@
       <c r="C15" s="40"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="I15" s="40"/>
+      <c r="H15" s="3"/>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
-      <c r="M15" s="42"/>
+      <c r="L15" s="40"/>
       <c r="N15" s="42"/>
       <c r="O15" s="42"/>
       <c r="P15" s="42"/>
       <c r="Q15" s="42"/>
-      <c r="Z15" s="3"/>
+      <c r="R15" s="42"/>
+      <c r="AA15" s="3"/>
     </row>
     <row r="16" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
@@ -2590,15 +2609,16 @@
       <c r="C16" s="40"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="I16" s="40"/>
+      <c r="H16" s="3"/>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
-      <c r="M16" s="42"/>
+      <c r="L16" s="40"/>
       <c r="N16" s="42"/>
       <c r="O16" s="42"/>
       <c r="P16" s="42"/>
       <c r="Q16" s="42"/>
-      <c r="Z16" s="3"/>
+      <c r="R16" s="42"/>
+      <c r="AA16" s="3"/>
     </row>
     <row r="17" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
@@ -2606,15 +2626,16 @@
       <c r="C17" s="40"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="I17" s="40"/>
+      <c r="H17" s="3"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
-      <c r="M17" s="42"/>
+      <c r="L17" s="40"/>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
-      <c r="Z17" s="3"/>
+      <c r="R17" s="42"/>
+      <c r="AA17" s="3"/>
     </row>
     <row r="18" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
@@ -2622,16 +2643,17 @@
       <c r="C18" s="40"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="I18" s="40"/>
+      <c r="H18" s="3"/>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
-      <c r="M18" s="42"/>
+      <c r="L18" s="40"/>
       <c r="N18" s="42"/>
       <c r="O18" s="42"/>
       <c r="P18" s="42"/>
       <c r="Q18" s="42"/>
-      <c r="Z18" s="3"/>
-      <c r="AI18" s="45"/>
+      <c r="R18" s="42"/>
+      <c r="AA18" s="3"/>
+      <c r="AJ18" s="45"/>
     </row>
     <row r="19" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="39"/>
@@ -2639,10 +2661,11 @@
       <c r="C19" s="40"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="I19" s="40"/>
+      <c r="H19" s="3"/>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
-      <c r="Z19" s="3"/>
+      <c r="L19" s="40"/>
+      <c r="AA19" s="3"/>
     </row>
     <row r="20" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
@@ -2650,10 +2673,11 @@
       <c r="C20" s="40"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="I20" s="40"/>
+      <c r="H20" s="3"/>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>
-      <c r="Z20" s="3"/>
+      <c r="L20" s="40"/>
+      <c r="AA20" s="3"/>
     </row>
     <row r="21" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
@@ -2661,10 +2685,11 @@
       <c r="C21" s="40"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="I21" s="40"/>
+      <c r="H21" s="3"/>
       <c r="J21" s="40"/>
       <c r="K21" s="40"/>
-      <c r="Z21" s="3"/>
+      <c r="L21" s="40"/>
+      <c r="AA21" s="3"/>
     </row>
     <row r="22" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="39"/>
@@ -2672,10 +2697,11 @@
       <c r="C22" s="40"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="I22" s="40"/>
+      <c r="H22" s="3"/>
       <c r="J22" s="40"/>
       <c r="K22" s="40"/>
-      <c r="Z22" s="3"/>
+      <c r="L22" s="40"/>
+      <c r="AA22" s="3"/>
     </row>
     <row r="23" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="39"/>
@@ -2683,10 +2709,11 @@
       <c r="C23" s="40"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="I23" s="40"/>
+      <c r="H23" s="3"/>
       <c r="J23" s="40"/>
       <c r="K23" s="40"/>
-      <c r="Z23" s="3"/>
+      <c r="L23" s="40"/>
+      <c r="AA23" s="3"/>
     </row>
     <row r="24" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39"/>
@@ -2694,10 +2721,11 @@
       <c r="C24" s="40"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="I24" s="40"/>
+      <c r="H24" s="3"/>
       <c r="J24" s="40"/>
       <c r="K24" s="40"/>
-      <c r="Z24" s="3"/>
+      <c r="L24" s="40"/>
+      <c r="AA24" s="3"/>
     </row>
     <row r="25" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39"/>
@@ -2705,10 +2733,11 @@
       <c r="C25" s="40"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="I25" s="40"/>
+      <c r="H25" s="3"/>
       <c r="J25" s="40"/>
       <c r="K25" s="40"/>
-      <c r="Z25" s="3"/>
+      <c r="L25" s="40"/>
+      <c r="AA25" s="3"/>
     </row>
     <row r="26" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
@@ -2716,10 +2745,11 @@
       <c r="C26" s="40"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="I26" s="40"/>
+      <c r="H26" s="3"/>
       <c r="J26" s="40"/>
       <c r="K26" s="40"/>
-      <c r="Z26" s="3"/>
+      <c r="L26" s="40"/>
+      <c r="AA26" s="3"/>
     </row>
     <row r="27" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
@@ -2727,10 +2757,11 @@
       <c r="C27" s="40"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="I27" s="40"/>
+      <c r="H27" s="3"/>
       <c r="J27" s="40"/>
       <c r="K27" s="40"/>
-      <c r="Z27" s="3"/>
+      <c r="L27" s="40"/>
+      <c r="AA27" s="3"/>
     </row>
     <row r="28" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="39"/>
@@ -2738,10 +2769,11 @@
       <c r="C28" s="40"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="I28" s="40"/>
+      <c r="H28" s="3"/>
       <c r="J28" s="40"/>
       <c r="K28" s="40"/>
-      <c r="Z28" s="3"/>
+      <c r="L28" s="40"/>
+      <c r="AA28" s="3"/>
     </row>
     <row r="29" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="39"/>
@@ -2749,10 +2781,11 @@
       <c r="C29" s="40"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="I29" s="40"/>
+      <c r="H29" s="3"/>
       <c r="J29" s="40"/>
       <c r="K29" s="40"/>
-      <c r="Z29" s="3"/>
+      <c r="L29" s="40"/>
+      <c r="AA29" s="3"/>
     </row>
     <row r="30" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="39"/>
@@ -2760,10 +2793,11 @@
       <c r="C30" s="40"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="I30" s="40"/>
+      <c r="H30" s="3"/>
       <c r="J30" s="40"/>
       <c r="K30" s="40"/>
-      <c r="Z30" s="3"/>
+      <c r="L30" s="40"/>
+      <c r="AA30" s="3"/>
     </row>
     <row r="31" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="39"/>
@@ -2771,10 +2805,11 @@
       <c r="C31" s="40"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="I31" s="40"/>
+      <c r="H31" s="3"/>
       <c r="J31" s="40"/>
       <c r="K31" s="40"/>
-      <c r="Z31" s="3"/>
+      <c r="L31" s="40"/>
+      <c r="AA31" s="3"/>
     </row>
     <row r="32" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39"/>
@@ -2782,10 +2817,11 @@
       <c r="C32" s="40"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="I32" s="40"/>
+      <c r="H32" s="3"/>
       <c r="J32" s="40"/>
       <c r="K32" s="40"/>
-      <c r="Z32" s="3"/>
+      <c r="L32" s="40"/>
+      <c r="AA32" s="3"/>
     </row>
     <row r="33" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="39"/>
@@ -2793,10 +2829,11 @@
       <c r="C33" s="40"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="I33" s="40"/>
+      <c r="H33" s="3"/>
       <c r="J33" s="40"/>
       <c r="K33" s="40"/>
-      <c r="Z33" s="3"/>
+      <c r="L33" s="40"/>
+      <c r="AA33" s="3"/>
     </row>
     <row r="34" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="39"/>
@@ -2804,10 +2841,11 @@
       <c r="C34" s="40"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="I34" s="40"/>
+      <c r="H34" s="3"/>
       <c r="J34" s="40"/>
       <c r="K34" s="40"/>
-      <c r="Z34" s="3"/>
+      <c r="L34" s="40"/>
+      <c r="AA34" s="3"/>
     </row>
     <row r="35" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="39"/>
@@ -2815,7 +2853,8 @@
       <c r="C35" s="40"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="Z35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="AA35" s="3"/>
     </row>
     <row r="36" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="39"/>
@@ -2823,7 +2862,8 @@
       <c r="C36" s="40"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="Z36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="AA36" s="3"/>
     </row>
     <row r="37" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="39"/>
@@ -2831,7 +2871,8 @@
       <c r="C37" s="40"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="Z37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="AA37" s="3"/>
     </row>
     <row r="38" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="39"/>
@@ -2839,7 +2880,8 @@
       <c r="C38" s="40"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="Z38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="AA38" s="3"/>
     </row>
     <row r="39" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="39"/>
@@ -2847,7 +2889,8 @@
       <c r="C39" s="40"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="Z39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="AA39" s="3"/>
     </row>
     <row r="40" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="39"/>
@@ -2855,7 +2898,8 @@
       <c r="C40" s="40"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="Z40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="AA40" s="3"/>
     </row>
     <row r="41" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="39"/>
@@ -2863,7 +2907,8 @@
       <c r="C41" s="40"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="Z41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="AA41" s="3"/>
     </row>
     <row r="42" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="39"/>
@@ -2871,7 +2916,8 @@
       <c r="C42" s="40"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="Z42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="AA42" s="3"/>
     </row>
     <row r="43" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="39"/>
@@ -2879,7 +2925,8 @@
       <c r="C43" s="40"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="Z43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="AA43" s="3"/>
     </row>
     <row r="44" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="39"/>
@@ -2887,7 +2934,8 @@
       <c r="C44" s="40"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="Z44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="AA44" s="3"/>
     </row>
     <row r="45" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="39"/>
@@ -2895,7 +2943,8 @@
       <c r="C45" s="40"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
-      <c r="Z45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="AA45" s="3"/>
     </row>
     <row r="46" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="39"/>
@@ -2903,7 +2952,8 @@
       <c r="C46" s="40"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="Z46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="AA46" s="3"/>
     </row>
     <row r="47" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="39"/>
@@ -2911,7 +2961,8 @@
       <c r="C47" s="40"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="Z47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="AA47" s="3"/>
     </row>
     <row r="48" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="39"/>
@@ -2919,7 +2970,8 @@
       <c r="C48" s="40"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="Z48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="AA48" s="3"/>
     </row>
     <row r="49" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="39"/>
@@ -2927,15 +2979,16 @@
       <c r="C49" s="40"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="Z49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="AA49" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L7:L14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M7:M14" type="list">
       <formula1>'MBE chamber env'!$D$7:$D$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J48" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K48" type="list">
       <formula1>'MBE chamber env'!$J$8:$J$13</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2957,7 +3010,7 @@
   </sheetPr>
   <dimension ref="A1:AR35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2986,29 +3039,29 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="50" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="50" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
@@ -3045,7 +3098,7 @@
     </row>
     <row r="2" s="55" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -3053,13 +3106,13 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
@@ -3099,16 +3152,16 @@
     </row>
     <row r="3" s="58" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -3153,16 +3206,16 @@
     </row>
     <row r="4" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -3207,30 +3260,30 @@
     </row>
     <row r="5" s="53" customFormat="true" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="67"/>
       <c r="G5" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H5" s="68"/>
       <c r="I5" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K5" s="67"/>
       <c r="L5" s="67"/>
@@ -3269,43 +3322,43 @@
     </row>
     <row r="6" s="70" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H6" s="70" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N6" s="34"/>
       <c r="O6" s="34"/>
@@ -3341,13 +3394,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C7" s="71" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E7" s="48" t="n">
         <v>4</v>
@@ -3356,23 +3409,23 @@
         <v>1</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H7" s="49" t="n">
         <v>0.1</v>
       </c>
       <c r="I7" s="73" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J7" s="73"/>
       <c r="K7" s="73" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L7" s="73" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M7" s="73" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N7" s="73"/>
       <c r="O7" s="73"/>
@@ -3391,13 +3444,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E8" s="48" t="n">
         <v>4</v>
@@ -3406,19 +3459,19 @@
         <v>2</v>
       </c>
       <c r="G8" s="73" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H8" s="49" t="n">
         <v>0.05</v>
       </c>
       <c r="I8" s="73" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K8" s="75" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L8" s="75" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M8" s="73"/>
       <c r="N8" s="73"/>
@@ -3430,13 +3483,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="47" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D9" s="72" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E9" s="48" t="n">
         <v>4</v>
@@ -3445,17 +3498,17 @@
         <v>1</v>
       </c>
       <c r="I9" s="73" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J9" s="73"/>
       <c r="K9" s="73" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L9" s="73" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M9" s="48" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="O9" s="76"/>
       <c r="P9" s="76"/>
@@ -3464,13 +3517,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="47" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C10" s="71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E10" s="48" t="n">
         <v>4</v>
@@ -3480,13 +3533,13 @@
       </c>
       <c r="G10" s="71"/>
       <c r="I10" s="73" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K10" s="75" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L10" s="75" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="O10" s="76"/>
       <c r="P10" s="76"/>
@@ -3706,7 +3759,7 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3728,76 +3781,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J1" s="79"/>
     </row>
     <row r="2" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="80" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="81" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" s="82"/>
     </row>
     <row r="3" s="58" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="83"/>
     </row>
     <row r="4" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J4" s="84"/>
     </row>
     <row r="5" s="86" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="85" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J5" s="87"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="88" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D6" s="89" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E6" s="89" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F6" s="89" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G6" s="89" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H6" s="89"/>
       <c r="I6" s="89"/>
@@ -3807,22 +3860,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="49" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E7" s="91" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="J7" s="91"/>
       <c r="K7" s="91"/>
@@ -3867,7 +3920,7 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3890,21 +3943,21 @@
     </row>
     <row r="2" s="96" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="94" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="94"/>
       <c r="C2" s="94"/>
       <c r="D2" s="94"/>
       <c r="E2" s="95" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="95" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" s="97" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3914,7 +3967,7 @@
     </row>
     <row r="4" s="100" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="98" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="98"/>
       <c r="C4" s="98"/>
@@ -3924,7 +3977,7 @@
     </row>
     <row r="5" s="101" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="85" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3934,28 +3987,28 @@
     </row>
     <row r="6" s="102" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="70" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="70"/>
       <c r="C6" s="70" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D6" s="70" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E6" s="70" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F6" s="70" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>1</v>
@@ -3982,7 +4035,7 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4001,185 +4054,185 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" s="55" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="55" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="55" t="s">
-        <v>28</v>
-      </c>
       <c r="I2" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="55" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="55" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" s="58" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E3" s="57"/>
       <c r="F3" s="58" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G3" s="58" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" s="65" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E4" s="59"/>
     </row>
     <row r="5" s="86" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="67"/>
     </row>
     <row r="6" s="70" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F6" s="70" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G6" s="70" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H6" s="70" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I6" s="70" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J6" s="70" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="46"/>
       <c r="B7" s="47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C7" s="71" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E7" s="72"/>
       <c r="F7" s="3" t="n">
         <v>456</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="46"/>
       <c r="B8" s="47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E8" s="72"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="46"/>
       <c r="B9" s="47" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D9" s="72" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E9" s="72"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="46"/>
       <c r="B10" s="47" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C10" s="71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E10" s="72"/>
     </row>
@@ -4208,7 +4261,7 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -4225,47 +4278,47 @@
     </row>
     <row r="2" s="54" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" s="57" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" s="60" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" s="68" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="85" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" s="70" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="70" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D6" s="70" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="49" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added features and linting
</commit_message>
<xml_diff>
--- a/tests/data/mbe/2023_06_12/MBE8_config.xlsx
+++ b/tests/data/mbe/2023_06_12/MBE8_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MBE sources" sheetId="1" state="visible" r:id="rId3"/>
@@ -661,7 +661,7 @@
     <t xml:space="preserve">bep_unit</t>
   </si>
   <si>
-    <t xml:space="preserve">GC Igd.PG.MV</t>
+    <t xml:space="preserve">GC IGd.PG.MV</t>
   </si>
   <si>
     <t xml:space="preserve">mbar</t>
@@ -737,7 +737,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
@@ -747,7 +747,6 @@
     <numFmt numFmtId="170" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="171" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="172" formatCode="0.00E+00"/>
-    <numFmt numFmtId="173" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -960,7 +959,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="115">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1277,28 +1276,124 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1307,66 +1402,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1636,7 +1671,7 @@
   </sheetPr>
   <dimension ref="A1:AZ49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -3819,149 +3854,148 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="3" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="3" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="79" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="2" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="2" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="50" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="81" customFormat="true" ht="101.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="79"/>
-    </row>
-    <row r="2" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="80" t="s">
+      <c r="J1" s="82"/>
+    </row>
+    <row r="2" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="82"/>
-    </row>
-    <row r="3" s="58" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="J2" s="85"/>
+    </row>
+    <row r="3" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="83"/>
-    </row>
-    <row r="4" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="J3" s="88"/>
+    </row>
+    <row r="4" s="90" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="84"/>
-    </row>
-    <row r="5" s="86" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="85" t="s">
+      <c r="J4" s="91"/>
+    </row>
+    <row r="5" s="93" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="87"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="88" t="s">
+      <c r="J5" s="94"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="96" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="89" t="s">
+      <c r="C6" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="96" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="89" t="s">
+      <c r="E6" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="89" t="s">
+      <c r="F6" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="89" t="s">
+      <c r="G6" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="98" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="99" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="99" t="s">
         <v>159</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
+      <c r="C8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="91"/>
+      <c r="C9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
+      <c r="C10" s="99"/>
+      <c r="E10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3992,31 +4026,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="1" s="94" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="101" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-    </row>
-    <row r="2" s="97" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="95" t="s">
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+    </row>
+    <row r="2" s="104" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="96" t="s">
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="103" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" s="98" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="105" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
@@ -4026,27 +4060,27 @@
       <c r="E3" s="58"/>
       <c r="F3" s="58"/>
     </row>
-    <row r="4" s="101" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="99" t="s">
+    <row r="4" s="108" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-    </row>
-    <row r="5" s="102" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="85" t="s">
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+    </row>
+    <row r="5" s="111" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="109" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-    </row>
-    <row r="6" s="103" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+    </row>
+    <row r="6" s="112" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="70" t="s">
         <v>41</v>
       </c>
@@ -4189,7 +4223,7 @@
       </c>
       <c r="E4" s="59"/>
     </row>
-    <row r="5" s="86" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="110" customFormat="true" ht="38.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
         <v>39</v>
       </c>
@@ -4247,7 +4281,7 @@
       <c r="D7" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="113" t="s">
         <v>176</v>
       </c>
       <c r="F7" s="3" t="n">
@@ -4277,7 +4311,7 @@
       <c r="D8" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="104" t="s">
+      <c r="E8" s="113" t="s">
         <v>176</v>
       </c>
       <c r="F8" s="3" t="n">
@@ -4307,7 +4341,7 @@
       <c r="D9" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="113" t="s">
         <v>176</v>
       </c>
       <c r="F9" s="3" t="n">
@@ -4337,7 +4371,7 @@
       <c r="D10" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="113" t="s">
         <v>176</v>
       </c>
       <c r="F10" s="3" t="n">
@@ -4391,7 +4425,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="105" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="114" width="14.06"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="49" width="11.53"/>
   </cols>
   <sheetData>
@@ -4416,7 +4450,7 @@
       </c>
     </row>
     <row r="5" s="68" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="109" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>